<commit_message>
process executive data in test2.py
</commit_message>
<xml_diff>
--- a/Data/aging_stock_summary.xlsx
+++ b/Data/aging_stock_summary.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL13"/>
+  <dimension ref="A1:AL12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,7 +629,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Within 15 Days</t>
+          <t>Expired</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -685,12 +685,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Within 15 Days</t>
+          <t>Within 30 Days</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Naprox</t>
+          <t>Flucloxin</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -698,12 +698,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Naprox Plus 500mg Tablet - 36's</t>
+          <t>Flucloxin 100ml Dry Suspension</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>22</v>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -721,9 +723,7 @@
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="n">
-        <v>2</v>
-      </c>
+      <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr"/>
@@ -741,12 +741,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Within 15 Days</t>
+          <t>Within 30 Days</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Toperin</t>
+          <t>Flucloxin</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -754,15 +754,15 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Toperin 50mg Tablet - 60's</t>
+          <t>Flucloxin 500mg Capsule 40's</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>19</v>
-      </c>
+      <c r="G4" t="n">
+        <v>7</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
@@ -779,7 +779,9 @@
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
+      <c r="Y4" t="n">
+        <v>1</v>
+      </c>
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr"/>
@@ -797,12 +799,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Within 15 Days</t>
+          <t>Within 30 Days</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Zithrox</t>
+          <t>Mebidal</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -810,7 +812,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Zithrox 50ml Powder for Suspension</t>
+          <t>Mebidal Tablet</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -829,9 +831,7 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
-      <c r="U5" t="n">
-        <v>344</v>
-      </c>
+      <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
@@ -839,7 +839,9 @@
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
+      <c r="AC5" t="n">
+        <v>24</v>
+      </c>
       <c r="AD5" t="inlineStr"/>
       <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
@@ -853,12 +855,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Within 15 Days</t>
+          <t>Within 30 Days</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Zithrox</t>
+          <t>Naprox</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -866,7 +868,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Zithrox 20ml Powder for Suspension</t>
+          <t>Naprox Plus 500mg Tablet - 36's</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -877,9 +879,7 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
-        <v>3</v>
-      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
@@ -891,7 +891,9 @@
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
+      <c r="Y6" t="n">
+        <v>1</v>
+      </c>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
@@ -909,12 +911,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Within 60 Days</t>
+          <t>Within 30 Days</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Flucloxin</t>
+          <t>Osticare</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -922,17 +924,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Flucloxin 100ml Dry Suspension</t>
+          <t>Osticare Tablet 30's</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>22</v>
-      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
@@ -947,7 +949,9 @@
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
+      <c r="Y7" t="n">
+        <v>1</v>
+      </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
@@ -970,7 +974,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Flucloxin</t>
+          <t>Oradin</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -978,17 +982,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Flucloxin 500mg Capsule 40's</t>
+          <t>Oradin 60ml Suspension</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>7</v>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>2</v>
+      </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
@@ -1003,9 +1007,7 @@
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="n">
-        <v>1</v>
-      </c>
+      <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
@@ -1023,12 +1025,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Within 60 Days</t>
+          <t>Within 90 Days</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mebidal</t>
+          <t>Dinafex</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -1036,7 +1038,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Mebidal Tablet</t>
+          <t>Dinafex 50ml Suspension</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -1064,7 +1066,7 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="AD9" t="inlineStr"/>
       <c r="AE9" t="inlineStr"/>
@@ -1079,7 +1081,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Within 60 Days</t>
+          <t>Within 90 Days</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1101,7 +1103,7 @@
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -1135,12 +1137,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Within 60 Days</t>
+          <t>Within 90 Days</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Osticare</t>
+          <t>Toti</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -1148,16 +1150,18 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Osticare Tablet 30's</t>
+          <t>Toti 100ml Syrup</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>14</v>
+      </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -1173,11 +1177,11 @@
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="n">
-        <v>1</v>
-      </c>
+      <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
+      <c r="AA11" t="n">
+        <v>33</v>
+      </c>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="inlineStr"/>
@@ -1198,7 +1202,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Oradin</t>
+          <t>Zithrox</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1206,7 +1210,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Oradin 60ml Suspension</t>
+          <t>Zithrox 35ml Dry Suspension</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -1215,7 +1219,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
@@ -1231,7 +1235,9 @@
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
+      <c r="Y12" t="n">
+        <v>1</v>
+      </c>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr"/>
@@ -1246,62 +1252,6 @@
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr"/>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Within 90 Days</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Toti</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Toti 100ml Syrup</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="n">
-        <v>14</v>
-      </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="inlineStr"/>
-      <c r="AI13" t="inlineStr"/>
-      <c r="AJ13" t="inlineStr"/>
-      <c r="AK13" t="inlineStr"/>
-      <c r="AL13" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>